<commit_message>
cleaned up scripts. added to .gitignore file
</commit_message>
<xml_diff>
--- a/data/sr-active-extract.xlsx
+++ b/data/sr-active-extract.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Request List" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Request List'!$A$1:$P$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Request List'!$A$1:$P$64</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="244">
   <si>
     <t>Id</t>
   </si>
@@ -263,10 +263,40 @@
     <t>plasmalyte 148 and 10% glucose changes to glucose 0% upon verification</t>
   </si>
   <si>
-    <t>210832</t>
-  </si>
-  <si>
-    <t>[INFUSIONS] - ifosfamide disappearing off MAR before complete.</t>
+    <t>215632</t>
+  </si>
+  <si>
+    <t>Clinic would like to have all staff recipients of results (Send to YPHS pool)</t>
+  </si>
+  <si>
+    <t>Parrott, Christine</t>
+  </si>
+  <si>
+    <t>EMR App - Ambulatory &amp; Portals</t>
+  </si>
+  <si>
+    <t>216717</t>
+  </si>
+  <si>
+    <t>ANZNN Surg Extract 2017</t>
+  </si>
+  <si>
+    <t>Nutley, Julia</t>
+  </si>
+  <si>
+    <t>Voskoboynik, Alice</t>
+  </si>
+  <si>
+    <t>217319</t>
+  </si>
+  <si>
+    <t>ANZNN Cong Abnorm Extract 2017 &amp; Table Abstraction</t>
+  </si>
+  <si>
+    <t>221212</t>
+  </si>
+  <si>
+    <t>EMR BEACON - 6MP issue</t>
   </si>
   <si>
     <t>Cochrane, Emma</t>
@@ -278,420 +308,330 @@
     <t>EMR App - Beacon</t>
   </si>
   <si>
-    <t>211113</t>
-  </si>
-  <si>
-    <t>[INFUSIONS] - no methotrexate row</t>
+    <t>228723</t>
+  </si>
+  <si>
+    <t>Rover Charging Station Required</t>
+  </si>
+  <si>
+    <t>Davidson, Kirsten</t>
+  </si>
+  <si>
+    <t>Lloyd, Matthew</t>
+  </si>
+  <si>
+    <t>EMR Technical - Infrastructure</t>
+  </si>
+  <si>
+    <t>232650</t>
+  </si>
+  <si>
+    <t>EMR willow verifying issue - G5%, 0.9%NaCl, 60 K</t>
+  </si>
+  <si>
+    <t>Kouw, Sarah</t>
+  </si>
+  <si>
+    <t>235455</t>
+  </si>
+  <si>
+    <t>[sherlock 3027771] Inpatient visit charges being sent to Impulse</t>
+  </si>
+  <si>
+    <t>Thomas, Anu</t>
+  </si>
+  <si>
+    <t>236023</t>
+  </si>
+  <si>
+    <t>Scheduling Reports access for CPMS (Children's Pain Management Service) Medical cliniicians.</t>
+  </si>
+  <si>
+    <t>Doran, Blaise</t>
+  </si>
+  <si>
+    <t>243378</t>
+  </si>
+  <si>
+    <t>Referrals linking to Cancelled/DNA appts</t>
+  </si>
+  <si>
+    <t>248123</t>
+  </si>
+  <si>
+    <t>CCC Tissue Bank orders in theatre print to the wrong printer/different printer than other theatre tests</t>
+  </si>
+  <si>
+    <t>Burns, Kathleen</t>
+  </si>
+  <si>
+    <t>Sharma, Sumit</t>
+  </si>
+  <si>
+    <t>EMR App - Optime</t>
+  </si>
+  <si>
+    <t>250814</t>
+  </si>
+  <si>
+    <t>EMR-Cadence/Priya Nair(Impulse)- Referral used to bill another department</t>
+  </si>
+  <si>
+    <t>Flask, Heather</t>
+  </si>
+  <si>
+    <t>Adem, Bilge</t>
+  </si>
+  <si>
+    <t>251098</t>
+  </si>
+  <si>
+    <t>Referral Starts &amp; Expiry Dates populated in error</t>
+  </si>
+  <si>
+    <t>254661</t>
+  </si>
+  <si>
+    <t>EMR access for Honoraries and Affiliates</t>
+  </si>
+  <si>
+    <t>Mantovani, Athena</t>
+  </si>
+  <si>
+    <t>Segal, Ahuva</t>
+  </si>
+  <si>
+    <t>EMR App - Research</t>
+  </si>
+  <si>
+    <t>263129</t>
+  </si>
+  <si>
+    <t>New daily report required for TAC public billings</t>
+  </si>
+  <si>
+    <t>264153</t>
+  </si>
+  <si>
+    <t>EPIC/IMPULSE- referral from EPIC not coming across to Impulse with provider number- Priya Nair and Bilge Adem</t>
+  </si>
+  <si>
+    <t>272408</t>
+  </si>
+  <si>
+    <t>1969 Hospital Chart Completion messages need resolution</t>
+  </si>
+  <si>
+    <t>Mechinaud, Francoise</t>
+  </si>
+  <si>
+    <t>274968</t>
+  </si>
+  <si>
+    <t>Clinicians requiring a 'reason' code(VISIT TYPE) for scheduling School Visits in Children's Pain Management Service.</t>
+  </si>
+  <si>
+    <t>276660</t>
+  </si>
+  <si>
+    <t>add details of surgical procedure and dates of procedure to Inpatient summary for medical staff</t>
+  </si>
+  <si>
+    <t>Palmer, Greta</t>
+  </si>
+  <si>
+    <t>288994</t>
+  </si>
+  <si>
+    <t>Review printout of discharge summary</t>
+  </si>
+  <si>
+    <t>Melchiori, Tristan</t>
+  </si>
+  <si>
+    <t>Tan, Adrian</t>
+  </si>
+  <si>
+    <t>EMR App - ClinDoc</t>
+  </si>
+  <si>
+    <t>290992</t>
+  </si>
+  <si>
+    <t>[Cadence] Replacement Referral Interaction</t>
+  </si>
+  <si>
+    <t>293601</t>
+  </si>
+  <si>
+    <t>Day Cancer Care Scheduled appointments status displays "Exam xxx" instead of "Arrived" when checking in</t>
+  </si>
+  <si>
+    <t>Clemens, Theresa</t>
   </si>
   <si>
     <t>Stewart, Aimee</t>
   </si>
   <si>
-    <t>215632</t>
-  </si>
-  <si>
-    <t>Clinic would like to have all staff recipients of results (Send to YPHS pool)</t>
-  </si>
-  <si>
-    <t>Parrott, Christine</t>
-  </si>
-  <si>
-    <t>EMR App - Ambulatory &amp; Portals</t>
-  </si>
-  <si>
-    <t>216717</t>
-  </si>
-  <si>
-    <t>ANZNN Surg Extract 2017</t>
-  </si>
-  <si>
-    <t>Nutley, Julia</t>
-  </si>
-  <si>
-    <t>Voskoboynik, Alice</t>
-  </si>
-  <si>
-    <t>217319</t>
-  </si>
-  <si>
-    <t>ANZNN Cong Abnorm Extract 2017 &amp; Table Abstraction</t>
-  </si>
-  <si>
-    <t>221212</t>
-  </si>
-  <si>
-    <t>EMR BEACON - 6MP issue</t>
-  </si>
-  <si>
-    <t>224580</t>
-  </si>
-  <si>
-    <t>scheduled orders report</t>
+    <t>309582</t>
+  </si>
+  <si>
+    <t>[Cadence] Wait List Contact Error</t>
+  </si>
+  <si>
+    <t>309584</t>
+  </si>
+  <si>
+    <t>Access_log primary Key conversion in TST</t>
+  </si>
+  <si>
+    <t>Singh, Sunita</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>314149</t>
+  </si>
+  <si>
+    <t>DR - Disaster Recovery - Cache replication</t>
+  </si>
+  <si>
+    <t>La Fortezza, Enzo</t>
+  </si>
+  <si>
+    <t>Omarjee, Bilal</t>
+  </si>
+  <si>
+    <t>ICT DBA</t>
+  </si>
+  <si>
+    <t>315171</t>
+  </si>
+  <si>
+    <t>incorrect fax number</t>
+  </si>
+  <si>
+    <t>Ternes, Anne-Marie</t>
+  </si>
+  <si>
+    <t>Kaye, Linnea</t>
+  </si>
+  <si>
+    <t>328758</t>
+  </si>
+  <si>
+    <t>review URs for merge</t>
+  </si>
+  <si>
+    <t>High - Severity 2</t>
+  </si>
+  <si>
+    <t>Cassin, Kathy</t>
+  </si>
+  <si>
+    <t>331097</t>
+  </si>
+  <si>
+    <t>no order for amiodarone powders</t>
+  </si>
+  <si>
+    <t>336351</t>
+  </si>
+  <si>
+    <t>Neurodevelopment and Disability physicians would like notification of patients who cancel appointments</t>
+  </si>
+  <si>
+    <t>Sutherland, Ingrid</t>
+  </si>
+  <si>
+    <t>336399</t>
+  </si>
+  <si>
+    <t>Cancer Services Seps, Beddays, ALOS etc. regular report</t>
+  </si>
+  <si>
+    <t>Gilbertson, Heather</t>
+  </si>
+  <si>
+    <t>Horsburgh, Tracy</t>
+  </si>
+  <si>
+    <t>341021</t>
+  </si>
+  <si>
+    <t>Metabolic team require new prescription products to be on system for prescribing</t>
+  </si>
+  <si>
+    <t>Normoyle, Mia</t>
+  </si>
+  <si>
+    <t>342739</t>
+  </si>
+  <si>
+    <t>[cadence] changes to public waiting list report</t>
   </si>
   <si>
     <t>Russell, Natasha</t>
   </si>
   <si>
+    <t>345032</t>
+  </si>
+  <si>
+    <t>need for script tray in printer</t>
+  </si>
+  <si>
+    <t>Fullerton, Jess</t>
+  </si>
+  <si>
+    <t>Fellowes, Luke</t>
+  </si>
+  <si>
+    <t>349184</t>
+  </si>
+  <si>
+    <t>Screen shot of relevant page in Results Review -  in regards to the Compliance reports</t>
+  </si>
+  <si>
+    <t>Jones, Sueellan</t>
+  </si>
+  <si>
+    <t>Pending end user</t>
+  </si>
+  <si>
+    <t>350019</t>
+  </si>
+  <si>
+    <t>Assistance with status boards on Haiku</t>
+  </si>
+  <si>
+    <t>Sivakumar, Harry</t>
+  </si>
+  <si>
+    <t>Gehrz, Casie</t>
+  </si>
+  <si>
+    <t>354197</t>
+  </si>
+  <si>
+    <t>New ophthalmology theatre order sets</t>
+  </si>
+  <si>
+    <t>Lewis, Catherine</t>
+  </si>
+  <si>
+    <t>EMR Ordersets</t>
+  </si>
+  <si>
+    <t>356171</t>
+  </si>
+  <si>
+    <t>New Visit Type for Day Cancer Care Nurse Education</t>
+  </si>
+  <si>
     <t>Tucker, Stephen</t>
   </si>
   <si>
-    <t>228723</t>
-  </si>
-  <si>
-    <t>Rover Charging Station Required</t>
-  </si>
-  <si>
-    <t>Davidson, Kirsten</t>
-  </si>
-  <si>
-    <t>Lloyd, Matthew</t>
-  </si>
-  <si>
-    <t>EMR Technical - Infrastructure</t>
-  </si>
-  <si>
-    <t>232650</t>
-  </si>
-  <si>
-    <t>EMR willow verifying issue - G5%, 0.9%NaCl, 60 K</t>
-  </si>
-  <si>
-    <t>Kouw, Sarah</t>
-  </si>
-  <si>
-    <t>235455</t>
-  </si>
-  <si>
-    <t>[sherlock 3027771] Inpatient visit charges being sent to Impulse</t>
-  </si>
-  <si>
-    <t>Thomas, Anu</t>
-  </si>
-  <si>
-    <t>236023</t>
-  </si>
-  <si>
-    <t>Scheduling Reports access for CPMS (Children's Pain Management Service) Medical cliniicians.</t>
-  </si>
-  <si>
-    <t>Doran, Blaise</t>
-  </si>
-  <si>
-    <t>243378</t>
-  </si>
-  <si>
-    <t>Referrals linking to Cancelled/DNA appts</t>
-  </si>
-  <si>
-    <t>248123</t>
-  </si>
-  <si>
-    <t>CCC Tissue Bank orders in theatre print to the wrong printer/different printer than other theatre tests</t>
-  </si>
-  <si>
-    <t>Burns, Kathleen</t>
-  </si>
-  <si>
-    <t>Sharma, Sumit</t>
-  </si>
-  <si>
-    <t>EMR App - Optime</t>
-  </si>
-  <si>
-    <t>250814</t>
-  </si>
-  <si>
-    <t>EMR-Cadence/Priya Nair(Impulse)- Referral used to bill another department</t>
-  </si>
-  <si>
-    <t>Flask, Heather</t>
-  </si>
-  <si>
-    <t>Adem, Bilge</t>
-  </si>
-  <si>
-    <t>251098</t>
-  </si>
-  <si>
-    <t>Referral Starts &amp; Expiry Dates populated in error</t>
-  </si>
-  <si>
-    <t>254190</t>
-  </si>
-  <si>
-    <t>[INFUSIONS] - Laronidase falling off flowsheet</t>
-  </si>
-  <si>
-    <t>254661</t>
-  </si>
-  <si>
-    <t>EMR access for Honoraries and Affiliates</t>
-  </si>
-  <si>
-    <t>Mantovani, Athena</t>
-  </si>
-  <si>
-    <t>Segal, Ahuva</t>
-  </si>
-  <si>
-    <t>EMR App - Research</t>
-  </si>
-  <si>
-    <t>262981</t>
-  </si>
-  <si>
-    <t>BEACON BUSULFAN PHARMACOKINETC Lab Order</t>
-  </si>
-  <si>
-    <t>Felmingham, Ben</t>
-  </si>
-  <si>
-    <t>263129</t>
-  </si>
-  <si>
-    <t>New daily report required for TAC public billings</t>
-  </si>
-  <si>
-    <t>264153</t>
-  </si>
-  <si>
-    <t>EPIC/IMPULSE- referral from EPIC not coming across to Impulse with provider number- Priya Nair and Bilge Adem</t>
-  </si>
-  <si>
-    <t>272408</t>
-  </si>
-  <si>
-    <t>1969 Hospital Chart Completion messages need resolution</t>
-  </si>
-  <si>
-    <t>Mechinaud, Francoise</t>
-  </si>
-  <si>
-    <t>274968</t>
-  </si>
-  <si>
-    <t>Clinicians requiring a 'reason' code(VISIT TYPE) for scheduling School Visits in Children's Pain Management Service.</t>
-  </si>
-  <si>
-    <t>276660</t>
-  </si>
-  <si>
-    <t>add details of surgical procedure and dates of procedure to Inpatient summary for medical staff</t>
-  </si>
-  <si>
-    <t>Palmer, Greta</t>
-  </si>
-  <si>
-    <t>280318</t>
-  </si>
-  <si>
-    <t>VINAH billing clinic for Day Medical Care</t>
-  </si>
-  <si>
-    <t>Goddard, James</t>
-  </si>
-  <si>
-    <t>283568</t>
-  </si>
-  <si>
-    <t>Updates to met navigator</t>
-  </si>
-  <si>
-    <t>Peterson, Anna</t>
-  </si>
-  <si>
-    <t>EMR App - ClinDoc</t>
-  </si>
-  <si>
-    <t>288994</t>
-  </si>
-  <si>
-    <t>Review printout of discharge summary</t>
-  </si>
-  <si>
-    <t>Melchiori, Tristan</t>
-  </si>
-  <si>
-    <t>Tan, Adrian</t>
-  </si>
-  <si>
-    <t>290992</t>
-  </si>
-  <si>
-    <t>[Cadence] Replacement Referral Interaction</t>
-  </si>
-  <si>
-    <t>293601</t>
-  </si>
-  <si>
-    <t>Day Cancer Care Scheduled appointments status displays "Exam xxx" instead of "Arrived" when checking in</t>
-  </si>
-  <si>
-    <t>Clemens, Theresa</t>
-  </si>
-  <si>
-    <t>309582</t>
-  </si>
-  <si>
-    <t>[Cadence] Wait List Contact Error</t>
-  </si>
-  <si>
-    <t>309584</t>
-  </si>
-  <si>
-    <t>Access_log primary Key conversion in TST</t>
-  </si>
-  <si>
-    <t>Singh, Sunita</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>314149</t>
-  </si>
-  <si>
-    <t>DR - Disaster Recovery - Cache replication</t>
-  </si>
-  <si>
-    <t>La Fortezza, Enzo</t>
-  </si>
-  <si>
-    <t>Omarjee, Bilal</t>
-  </si>
-  <si>
-    <t>ICT DBA</t>
-  </si>
-  <si>
-    <t>315171</t>
-  </si>
-  <si>
-    <t>incorrect fax number</t>
-  </si>
-  <si>
-    <t>Ternes, Anne-Marie</t>
-  </si>
-  <si>
-    <t>Kaye, Linnea</t>
-  </si>
-  <si>
-    <t>328758</t>
-  </si>
-  <si>
-    <t>review URs for merge</t>
-  </si>
-  <si>
-    <t>High - Severity 2</t>
-  </si>
-  <si>
-    <t>Cassin, Kathy</t>
-  </si>
-  <si>
-    <t>331097</t>
-  </si>
-  <si>
-    <t>no order for amiodarone powders</t>
-  </si>
-  <si>
-    <t>336149</t>
-  </si>
-  <si>
-    <t>Discharge summary report taking a long time to load</t>
-  </si>
-  <si>
-    <t>Luitingh, Taryn</t>
-  </si>
-  <si>
-    <t>336351</t>
-  </si>
-  <si>
-    <t>Neurodevelopment and Disability physicians would like notification of patients who cancel appointments</t>
-  </si>
-  <si>
-    <t>Sutherland, Ingrid</t>
-  </si>
-  <si>
-    <t>336399</t>
-  </si>
-  <si>
-    <t>Cancer Services Seps, Beddays, ALOS etc. regular report</t>
-  </si>
-  <si>
-    <t>Gilbertson, Heather</t>
-  </si>
-  <si>
-    <t>Horsburgh, Tracy</t>
-  </si>
-  <si>
-    <t>341021</t>
-  </si>
-  <si>
-    <t>Metabolic team require new prescription products to be on system for prescribing</t>
-  </si>
-  <si>
-    <t>Normoyle, Mia</t>
-  </si>
-  <si>
-    <t>342739</t>
-  </si>
-  <si>
-    <t>[cadence] changes to public waiting list report</t>
-  </si>
-  <si>
-    <t>345032</t>
-  </si>
-  <si>
-    <t>need for script tray in printer</t>
-  </si>
-  <si>
-    <t>Fullerton, Jess</t>
-  </si>
-  <si>
-    <t>Fellowes, Luke</t>
-  </si>
-  <si>
-    <t>349184</t>
-  </si>
-  <si>
-    <t>Screen shot of relevant page in Results Review -  in regards to the Compliance reports</t>
-  </si>
-  <si>
-    <t>Jones, Sueellan</t>
-  </si>
-  <si>
-    <t>Pending end user</t>
-  </si>
-  <si>
-    <t>350019</t>
-  </si>
-  <si>
-    <t>Assistance with status boards on Haiku</t>
-  </si>
-  <si>
-    <t>Sivakumar, Harry</t>
-  </si>
-  <si>
-    <t>Gehrz, Casie</t>
-  </si>
-  <si>
-    <t>354197</t>
-  </si>
-  <si>
-    <t>New ophthalmology theatre order sets</t>
-  </si>
-  <si>
-    <t>Lewis, Catherine</t>
-  </si>
-  <si>
-    <t>EMR Ordersets</t>
-  </si>
-  <si>
-    <t>356171</t>
-  </si>
-  <si>
-    <t>New Visit Type for Day Cancer Care Nurse Education</t>
-  </si>
-  <si>
     <t>358921</t>
   </si>
   <si>
@@ -722,115 +662,91 @@
     <t>Raymundo, Chin-Mae</t>
   </si>
   <si>
-    <t>361107</t>
-  </si>
-  <si>
-    <t>Report on PIV &amp; CVAD insertion and management documentation</t>
-  </si>
-  <si>
-    <t>Scott, Sue</t>
+    <t>363951</t>
+  </si>
+  <si>
+    <t>IT41509 apt booked not showing in qflow</t>
+  </si>
+  <si>
+    <t>Harker, Olivia</t>
+  </si>
+  <si>
+    <t>365820</t>
+  </si>
+  <si>
+    <t>Add EMR Providers 21/07</t>
+  </si>
+  <si>
+    <t>Richards, Shaun</t>
+  </si>
+  <si>
+    <t>368299</t>
+  </si>
+  <si>
+    <t>RCH portal access</t>
+  </si>
+  <si>
+    <t>Lockett, Kelly</t>
+  </si>
+  <si>
+    <t>Dorward, Sarah</t>
+  </si>
+  <si>
+    <t>368531</t>
+  </si>
+  <si>
+    <t>EPIC - Allergy blocks</t>
+  </si>
+  <si>
+    <t>Foster, Wendy</t>
+  </si>
+  <si>
+    <t>368692</t>
+  </si>
+  <si>
+    <t>PROTECT Study 36330</t>
+  </si>
+  <si>
+    <t>369182</t>
+  </si>
+  <si>
+    <t>[Waiting for response] Close encounter prompt to place f/up appt order if not discharging pt</t>
+  </si>
+  <si>
+    <t>Schoenmann, Casey</t>
+  </si>
+  <si>
+    <t>370218</t>
+  </si>
+  <si>
+    <t>Admin staff to have an all provider record for telephone encounters and documentaion</t>
+  </si>
+  <si>
+    <t>370705</t>
+  </si>
+  <si>
+    <t>Accreditation requirement Medical Imaging</t>
+  </si>
+  <si>
+    <t>Griffiths, Tania</t>
+  </si>
+  <si>
+    <t>372051</t>
+  </si>
+  <si>
+    <t>[Awaiting Signed Form] Data collection request out of the EMR for research project</t>
+  </si>
+  <si>
+    <t>Zhukova, Nataliya</t>
   </si>
   <si>
     <t>EMR Stage II Improvement</t>
   </si>
   <si>
-    <t>363951</t>
-  </si>
-  <si>
-    <t>IT41509 apt booked not showing in qflow</t>
-  </si>
-  <si>
-    <t>Harker, Olivia</t>
-  </si>
-  <si>
-    <t>365820</t>
-  </si>
-  <si>
-    <t>Add EMR Providers 21/07</t>
-  </si>
-  <si>
-    <t>Richards, Shaun</t>
-  </si>
-  <si>
-    <t>368299</t>
-  </si>
-  <si>
-    <t>RCH portal access</t>
-  </si>
-  <si>
-    <t>Lockett, Kelly</t>
-  </si>
-  <si>
-    <t>Dorward, Sarah</t>
-  </si>
-  <si>
-    <t>368692</t>
-  </si>
-  <si>
-    <t>PROTECT Study 36330</t>
-  </si>
-  <si>
-    <t>369182</t>
-  </si>
-  <si>
-    <t>Close encounter prompt to place f/up appt order if not discharging pt</t>
-  </si>
-  <si>
-    <t>Schoenmann, Casey</t>
-  </si>
-  <si>
-    <t>370218</t>
-  </si>
-  <si>
-    <t>Admin staff to have an all provider record for telephone encounters and documentaion</t>
-  </si>
-  <si>
-    <t>370669</t>
-  </si>
-  <si>
-    <t>Pop up appears when trying to sign future appointments in treatment plans</t>
-  </si>
-  <si>
-    <t>Sirianni, Nicole</t>
-  </si>
-  <si>
-    <t>370705</t>
-  </si>
-  <si>
-    <t>Accreditation requirement Medical Imaging</t>
-  </si>
-  <si>
-    <t>Griffiths, Tania</t>
-  </si>
-  <si>
-    <t>371281</t>
-  </si>
-  <si>
-    <t>DOXORUBICIN BEACON EURONET DOXORUBICIN</t>
-  </si>
-  <si>
-    <t>371285</t>
-  </si>
-  <si>
-    <t>Cadence Team - Update fleet resources on Snapboard</t>
-  </si>
-  <si>
-    <t>Bui, An</t>
-  </si>
-  <si>
-    <t>372045</t>
-  </si>
-  <si>
-    <t>EMR access</t>
-  </si>
-  <si>
-    <t>372051</t>
-  </si>
-  <si>
-    <t>[Awaiting Signed Form] Data collection request out of the EMR for research project</t>
-  </si>
-  <si>
-    <t>Zhukova, Nataliya</t>
+    <t>372465</t>
+  </si>
+  <si>
+    <t>EMR access-Monica Bhatia</t>
   </si>
 </sst>
 </file>
@@ -1629,11 +1545,11 @@
       </c>
       <c r="H16"/>
       <c r="I16" t="s" s="6">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s" s="6">
         <v>85</v>
       </c>
-      <c r="J16" t="s" s="6">
-        <v>86</v>
-      </c>
       <c r="K16" t="s" s="6">
         <v>24</v>
       </c>
@@ -1641,11 +1557,11 @@
         <v>10</v>
       </c>
       <c r="M16" t="n" s="7">
-        <v>42710.43869458333</v>
+        <v>42717.40797648148</v>
       </c>
       <c r="N16"/>
       <c r="O16" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P16" t="s" s="6">
         <v>26</v>
@@ -1653,17 +1569,17 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="6">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s" s="6">
         <v>87</v>
       </c>
-      <c r="B17" t="s" s="6">
-        <v>88</v>
-      </c>
       <c r="C17" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s" s="6">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s" s="6">
         <v>20</v>
@@ -1676,7 +1592,7 @@
         <v>89</v>
       </c>
       <c r="J17" t="s" s="6">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="K17" t="s" s="6">
         <v>24</v>
@@ -1685,11 +1601,11 @@
         <v>10</v>
       </c>
       <c r="M17" t="n" s="7">
-        <v>42710.42306931713</v>
+        <v>42719.47833268518</v>
       </c>
       <c r="N17"/>
       <c r="O17" t="s" s="6">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="P17" t="s" s="6">
         <v>26</v>
@@ -1703,11 +1619,11 @@
         <v>91</v>
       </c>
       <c r="C18" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s" s="6">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s" s="6">
         <v>20</v>
@@ -1717,10 +1633,10 @@
       </c>
       <c r="H18"/>
       <c r="I18" t="s" s="6">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="J18" t="s" s="6">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="K18" t="s" s="6">
         <v>24</v>
@@ -1729,11 +1645,11 @@
         <v>10</v>
       </c>
       <c r="M18" t="n" s="7">
-        <v>42717.40797648148</v>
+        <v>42719.41294297454</v>
       </c>
       <c r="N18"/>
       <c r="O18" t="s" s="6">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="P18" t="s" s="6">
         <v>26</v>
@@ -1741,17 +1657,17 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="6">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s" s="6">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s" s="6">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19" t="s" s="6">
         <v>20</v>
@@ -1761,10 +1677,10 @@
       </c>
       <c r="H19"/>
       <c r="I19" t="s" s="6">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s" s="6">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="K19" t="s" s="6">
         <v>24</v>
@@ -1773,11 +1689,11 @@
         <v>10</v>
       </c>
       <c r="M19" t="n" s="7">
-        <v>42719.47833268518</v>
+        <v>42726.48026793981</v>
       </c>
       <c r="N19"/>
       <c r="O19" t="s" s="6">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="P19" t="s" s="6">
         <v>26</v>
@@ -1785,17 +1701,17 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s" s="6">
         <v>98</v>
       </c>
-      <c r="B20" t="s" s="6">
-        <v>99</v>
-      </c>
       <c r="C20" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s" s="6">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F20" t="s" s="6">
         <v>20</v>
@@ -1805,10 +1721,10 @@
       </c>
       <c r="H20"/>
       <c r="I20" t="s" s="6">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J20" t="s" s="6">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="K20" t="s" s="6">
         <v>24</v>
@@ -1817,11 +1733,11 @@
         <v>10</v>
       </c>
       <c r="M20" t="n" s="7">
-        <v>42719.41294297454</v>
+        <v>42744.492281631945</v>
       </c>
       <c r="N20"/>
       <c r="O20" t="s" s="6">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="P20" t="s" s="6">
         <v>26</v>
@@ -1829,17 +1745,17 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="6">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s" s="6">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s" s="6">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s" s="6">
         <v>20</v>
@@ -1849,10 +1765,10 @@
       </c>
       <c r="H21"/>
       <c r="I21" t="s" s="6">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J21" t="s" s="6">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="K21" t="s" s="6">
         <v>24</v>
@@ -1861,7 +1777,7 @@
         <v>10</v>
       </c>
       <c r="M21" t="n" s="7">
-        <v>42726.48026793981</v>
+        <v>42751.56249019676</v>
       </c>
       <c r="N21"/>
       <c r="O21" t="s" s="6">
@@ -1873,17 +1789,17 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="6">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s" s="6">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s" s="6">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F22" t="s" s="6">
         <v>20</v>
@@ -1893,10 +1809,10 @@
       </c>
       <c r="H22"/>
       <c r="I22" t="s" s="6">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="J22" t="s" s="6">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="K22" t="s" s="6">
         <v>24</v>
@@ -1905,7 +1821,7 @@
         <v>10</v>
       </c>
       <c r="M22" t="n" s="7">
-        <v>42738.41012418982</v>
+        <v>42754.42458706019</v>
       </c>
       <c r="N22"/>
       <c r="O22" t="s" s="6">
@@ -1917,17 +1833,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="6">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s" s="6">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s" s="6">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s" s="6">
         <v>20</v>
@@ -1937,10 +1853,10 @@
       </c>
       <c r="H23"/>
       <c r="I23" t="s" s="6">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="J23" t="s" s="6">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="K23" t="s" s="6">
         <v>24</v>
@@ -1949,7 +1865,7 @@
         <v>10</v>
       </c>
       <c r="M23" t="n" s="7">
-        <v>42744.492281631945</v>
+        <v>42754.67374644676</v>
       </c>
       <c r="N23"/>
       <c r="O23" t="s" s="6">
@@ -1971,7 +1887,7 @@
       </c>
       <c r="D24"/>
       <c r="E24" t="s" s="6">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s" s="6">
         <v>20</v>
@@ -1981,10 +1897,10 @@
       </c>
       <c r="H24"/>
       <c r="I24" t="s" s="6">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="J24" t="s" s="6">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="K24" t="s" s="6">
         <v>24</v>
@@ -1993,7 +1909,7 @@
         <v>10</v>
       </c>
       <c r="M24" t="n" s="7">
-        <v>42751.56249019676</v>
+        <v>42768.39498278935</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="s" s="6">
@@ -2005,17 +1921,17 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="6">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s" s="6">
         <v>114</v>
       </c>
-      <c r="B25" t="s" s="6">
-        <v>115</v>
-      </c>
       <c r="C25" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s" s="6">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F25" t="s" s="6">
         <v>20</v>
@@ -2025,10 +1941,10 @@
       </c>
       <c r="H25"/>
       <c r="I25" t="s" s="6">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="J25" t="s" s="6">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="K25" t="s" s="6">
         <v>24</v>
@@ -2037,11 +1953,11 @@
         <v>10</v>
       </c>
       <c r="M25" t="n" s="7">
-        <v>42754.42458706019</v>
+        <v>42773.51863204861</v>
       </c>
       <c r="N25"/>
       <c r="O25" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P25" t="s" s="6">
         <v>26</v>
@@ -2049,17 +1965,17 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="6">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s" s="6">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s" s="6">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s" s="6">
         <v>20</v>
@@ -2069,10 +1985,10 @@
       </c>
       <c r="H26"/>
       <c r="I26" t="s" s="6">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="J26" t="s" s="6">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K26" t="s" s="6">
         <v>24</v>
@@ -2081,7 +1997,7 @@
         <v>10</v>
       </c>
       <c r="M26" t="n" s="7">
-        <v>42754.67374644676</v>
+        <v>42775.55602314815</v>
       </c>
       <c r="N26"/>
       <c r="O26" t="s" s="6">
@@ -2093,10 +2009,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="6">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s" s="6">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s" s="6">
         <v>18</v>
@@ -2109,12 +2025,10 @@
         <v>20</v>
       </c>
       <c r="G27" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H27"/>
-      <c r="I27" t="s" s="6">
-        <v>68</v>
-      </c>
+      <c r="I27"/>
       <c r="J27" t="s" s="6">
         <v>70</v>
       </c>
@@ -2125,7 +2039,7 @@
         <v>10</v>
       </c>
       <c r="M27" t="n" s="7">
-        <v>42768.39498278935</v>
+        <v>42775.608978460645</v>
       </c>
       <c r="N27"/>
       <c r="O27" t="s" s="6">
@@ -2137,17 +2051,17 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="6">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s" s="6">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s" s="6">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s" s="6">
         <v>20</v>
@@ -2157,10 +2071,10 @@
       </c>
       <c r="H28"/>
       <c r="I28" t="s" s="6">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J28" t="s" s="6">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K28" t="s" s="6">
         <v>24</v>
@@ -2169,11 +2083,11 @@
         <v>10</v>
       </c>
       <c r="M28" t="n" s="7">
-        <v>42773.51863204861</v>
+        <v>42781.63691741898</v>
       </c>
       <c r="N28"/>
       <c r="O28" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P28" t="s" s="6">
         <v>26</v>
@@ -2181,30 +2095,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="6">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s" s="6">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="s" s="6">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G29" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H29"/>
-      <c r="I29" t="s" s="6">
-        <v>130</v>
-      </c>
+      <c r="I29"/>
       <c r="J29" t="s" s="6">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="K29" t="s" s="6">
         <v>24</v>
@@ -2213,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="M29" t="n" s="7">
-        <v>42775.55602314815</v>
+        <v>42793.42732696759</v>
       </c>
       <c r="N29"/>
       <c r="O29" t="s" s="6">
@@ -2235,16 +2147,18 @@
       </c>
       <c r="D30"/>
       <c r="E30" t="s" s="6">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="F30" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G30" t="s" s="6">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H30"/>
-      <c r="I30"/>
+      <c r="I30" t="s" s="6">
+        <v>121</v>
+      </c>
       <c r="J30" t="s" s="6">
         <v>70</v>
       </c>
@@ -2255,7 +2169,7 @@
         <v>10</v>
       </c>
       <c r="M30" t="n" s="7">
-        <v>42775.608978460645</v>
+        <v>42794.396890104166</v>
       </c>
       <c r="N30"/>
       <c r="O30" t="s" s="6">
@@ -2277,20 +2191,18 @@
       </c>
       <c r="D31"/>
       <c r="E31" t="s" s="6">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="F31" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G31" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H31"/>
-      <c r="I31" t="s" s="6">
-        <v>89</v>
-      </c>
+      <c r="I31"/>
       <c r="J31" t="s" s="6">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K31" t="s" s="6">
         <v>24</v>
@@ -2299,11 +2211,11 @@
         <v>10</v>
       </c>
       <c r="M31" t="n" s="7">
-        <v>42781.56323396991</v>
+        <v>42803.527100300926</v>
       </c>
       <c r="N31"/>
       <c r="O31" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P31" t="s" s="6">
         <v>26</v>
@@ -2311,17 +2223,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="6">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s" s="6">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s" s="6">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="F32" t="s" s="6">
         <v>20</v>
@@ -2331,10 +2243,10 @@
       </c>
       <c r="H32"/>
       <c r="I32" t="s" s="6">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="J32" t="s" s="6">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="K32" t="s" s="6">
         <v>24</v>
@@ -2343,7 +2255,7 @@
         <v>10</v>
       </c>
       <c r="M32" t="n" s="7">
-        <v>42781.63691741898</v>
+        <v>42808.41914935185</v>
       </c>
       <c r="N32"/>
       <c r="O32" t="s" s="6">
@@ -2355,28 +2267,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="6">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s" s="6">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C33" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s" s="6">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F33" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G33" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33" t="s" s="6">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="K33" t="s" s="6">
         <v>24</v>
@@ -2385,7 +2297,7 @@
         <v>10</v>
       </c>
       <c r="M33" t="n" s="7">
-        <v>42790.591589351854</v>
+        <v>42809.75547043981</v>
       </c>
       <c r="N33"/>
       <c r="O33" t="s" s="6">
@@ -2397,28 +2309,30 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="6">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s" s="6">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D34"/>
       <c r="E34" t="s" s="6">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="F34" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G34" t="s" s="6">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H34"/>
-      <c r="I34"/>
+      <c r="I34" t="s" s="6">
+        <v>144</v>
+      </c>
       <c r="J34" t="s" s="6">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="K34" t="s" s="6">
         <v>24</v>
@@ -2427,7 +2341,7 @@
         <v>10</v>
       </c>
       <c r="M34" t="n" s="7">
-        <v>42793.42732696759</v>
+        <v>42825.42237341435</v>
       </c>
       <c r="N34"/>
       <c r="O34" t="s" s="6">
@@ -2439,17 +2353,17 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="6">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B35" t="s" s="6">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D35"/>
       <c r="E35" t="s" s="6">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="F35" t="s" s="6">
         <v>20</v>
@@ -2459,7 +2373,7 @@
       </c>
       <c r="H35"/>
       <c r="I35" t="s" s="6">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="J35" t="s" s="6">
         <v>70</v>
@@ -2471,7 +2385,7 @@
         <v>10</v>
       </c>
       <c r="M35" t="n" s="7">
-        <v>42794.396890104166</v>
+        <v>42829.463356238426</v>
       </c>
       <c r="N35"/>
       <c r="O35" t="s" s="6">
@@ -2483,28 +2397,30 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="6">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B36" t="s" s="6">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s" s="6">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G36" t="s" s="6">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H36"/>
-      <c r="I36"/>
+      <c r="I36" t="s" s="6">
+        <v>151</v>
+      </c>
       <c r="J36" t="s" s="6">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="K36" t="s" s="6">
         <v>24</v>
@@ -2513,11 +2429,11 @@
         <v>10</v>
       </c>
       <c r="M36" t="n" s="7">
-        <v>42803.527100300926</v>
+        <v>42832.56867890046</v>
       </c>
       <c r="N36"/>
       <c r="O36" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P36" t="s" s="6">
         <v>26</v>
@@ -2525,17 +2441,17 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="6">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s" s="6">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D37"/>
       <c r="E37" t="s" s="6">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="F37" t="s" s="6">
         <v>20</v>
@@ -2545,7 +2461,7 @@
       </c>
       <c r="H37"/>
       <c r="I37" t="s" s="6">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J37" t="s" s="6">
         <v>70</v>
@@ -2557,7 +2473,7 @@
         <v>10</v>
       </c>
       <c r="M37" t="n" s="7">
-        <v>42808.41914935185</v>
+        <v>42858.64125017361</v>
       </c>
       <c r="N37"/>
       <c r="O37" t="s" s="6">
@@ -2569,28 +2485,30 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="6">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s" s="6">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s" s="6">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G38" t="s" s="6">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H38"/>
-      <c r="I38"/>
+      <c r="I38" t="s" s="6">
+        <v>156</v>
+      </c>
       <c r="J38" t="s" s="6">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="K38" t="s" s="6">
         <v>24</v>
@@ -2599,29 +2517,29 @@
         <v>10</v>
       </c>
       <c r="M38" t="n" s="7">
-        <v>42809.75547043981</v>
+        <v>42857.6576828125</v>
       </c>
       <c r="N38"/>
       <c r="O38" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P38" t="s" s="6">
-        <v>26</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="6">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B39" t="s" s="6">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s" s="6">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F39" t="s" s="6">
         <v>20</v>
@@ -2631,10 +2549,10 @@
       </c>
       <c r="H39"/>
       <c r="I39" t="s" s="6">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="J39" t="s" s="6">
-        <v>70</v>
+        <v>162</v>
       </c>
       <c r="K39" t="s" s="6">
         <v>24</v>
@@ -2643,11 +2561,11 @@
         <v>10</v>
       </c>
       <c r="M39" t="n" s="7">
-        <v>42815.3946159375</v>
+        <v>42865.34305056713</v>
       </c>
       <c r="N39"/>
       <c r="O39" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P39" t="s" s="6">
         <v>26</v>
@@ -2655,17 +2573,17 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="6">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s" s="6">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C40" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D40"/>
       <c r="E40" t="s" s="6">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="F40" t="s" s="6">
         <v>20</v>
@@ -2675,10 +2593,10 @@
       </c>
       <c r="H40"/>
       <c r="I40" t="s" s="6">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="J40" t="s" s="6">
-        <v>161</v>
+        <v>70</v>
       </c>
       <c r="K40" t="s" s="6">
         <v>24</v>
@@ -2687,7 +2605,7 @@
         <v>10</v>
       </c>
       <c r="M40" t="n" s="7">
-        <v>42818.7020658912</v>
+        <v>42866.3875772338</v>
       </c>
       <c r="N40"/>
       <c r="O40" t="s" s="6">
@@ -2699,17 +2617,17 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="6">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s" s="6">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s" s="6">
-        <v>18</v>
+        <v>169</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s" s="6">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F41" t="s" s="6">
         <v>20</v>
@@ -2719,10 +2637,10 @@
       </c>
       <c r="H41"/>
       <c r="I41" t="s" s="6">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="J41" t="s" s="6">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="K41" t="s" s="6">
         <v>24</v>
@@ -2731,11 +2649,11 @@
         <v>10</v>
       </c>
       <c r="M41" t="n" s="7">
-        <v>42825.42237341435</v>
+        <v>42885.48330418982</v>
       </c>
       <c r="N41"/>
       <c r="O41" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P41" t="s" s="6">
         <v>26</v>
@@ -2743,17 +2661,17 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="6">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B42" t="s" s="6">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C42" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s" s="6">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F42" t="s" s="6">
         <v>20</v>
@@ -2763,10 +2681,10 @@
       </c>
       <c r="H42"/>
       <c r="I42" t="s" s="6">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="J42" t="s" s="6">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="K42" t="s" s="6">
         <v>24</v>
@@ -2775,7 +2693,7 @@
         <v>10</v>
       </c>
       <c r="M42" t="n" s="7">
-        <v>42829.463356238426</v>
+        <v>42887.53432255787</v>
       </c>
       <c r="N42"/>
       <c r="O42" t="s" s="6">
@@ -2787,17 +2705,17 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="6">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B43" t="s" s="6">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D43"/>
       <c r="E43" t="s" s="6">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F43" t="s" s="6">
         <v>20</v>
@@ -2807,10 +2725,10 @@
       </c>
       <c r="H43"/>
       <c r="I43" t="s" s="6">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="J43" t="s" s="6">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="K43" t="s" s="6">
         <v>24</v>
@@ -2819,11 +2737,11 @@
         <v>10</v>
       </c>
       <c r="M43" t="n" s="7">
-        <v>42832.56867890046</v>
+        <v>42894.3833237037</v>
       </c>
       <c r="N43"/>
       <c r="O43" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P43" t="s" s="6">
         <v>26</v>
@@ -2831,17 +2749,17 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="6">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B44" t="s" s="6">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C44" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D44"/>
       <c r="E44" t="s" s="6">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="F44" t="s" s="6">
         <v>20</v>
@@ -2851,10 +2769,10 @@
       </c>
       <c r="H44"/>
       <c r="I44" t="s" s="6">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="J44" t="s" s="6">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="K44" t="s" s="6">
         <v>24</v>
@@ -2863,7 +2781,7 @@
         <v>10</v>
       </c>
       <c r="M44" t="n" s="7">
-        <v>42858.64125017361</v>
+        <v>42894.63695923611</v>
       </c>
       <c r="N44"/>
       <c r="O44" t="s" s="6">
@@ -2875,17 +2793,17 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="6">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B45" t="s" s="6">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C45" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="s" s="6">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F45" t="s" s="6">
         <v>20</v>
@@ -2895,10 +2813,10 @@
       </c>
       <c r="H45"/>
       <c r="I45" t="s" s="6">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="J45" t="s" s="6">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="K45" t="s" s="6">
         <v>24</v>
@@ -2907,29 +2825,29 @@
         <v>10</v>
       </c>
       <c r="M45" t="n" s="7">
-        <v>42857.6576828125</v>
+        <v>42901.412132060184</v>
       </c>
       <c r="N45"/>
       <c r="O45" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P45" t="s" s="6">
-        <v>176</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="6">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B46" t="s" s="6">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D46"/>
       <c r="E46" t="s" s="6">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F46" t="s" s="6">
         <v>20</v>
@@ -2939,10 +2857,10 @@
       </c>
       <c r="H46"/>
       <c r="I46" t="s" s="6">
-        <v>180</v>
+        <v>68</v>
       </c>
       <c r="J46" t="s" s="6">
-        <v>181</v>
+        <v>70</v>
       </c>
       <c r="K46" t="s" s="6">
         <v>24</v>
@@ -2951,11 +2869,11 @@
         <v>10</v>
       </c>
       <c r="M46" t="n" s="7">
-        <v>42865.34305056713</v>
+        <v>42902.572656655095</v>
       </c>
       <c r="N46"/>
       <c r="O46" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P46" t="s" s="6">
         <v>26</v>
@@ -2963,17 +2881,17 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="6">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B47" t="s" s="6">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C47" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D47"/>
       <c r="E47" t="s" s="6">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F47" t="s" s="6">
         <v>20</v>
@@ -2983,10 +2901,10 @@
       </c>
       <c r="H47"/>
       <c r="I47" t="s" s="6">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J47" t="s" s="6">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="K47" t="s" s="6">
         <v>24</v>
@@ -2995,7 +2913,7 @@
         <v>10</v>
       </c>
       <c r="M47" t="n" s="7">
-        <v>42866.3875772338</v>
+        <v>42907.33971252315</v>
       </c>
       <c r="N47"/>
       <c r="O47" t="s" s="6">
@@ -3007,30 +2925,28 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="6">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B48" t="s" s="6">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C48" t="s" s="6">
-        <v>188</v>
+        <v>18</v>
       </c>
       <c r="D48"/>
       <c r="E48" t="s" s="6">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F48" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G48" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H48"/>
-      <c r="I48" t="s" s="6">
-        <v>189</v>
-      </c>
+      <c r="I48"/>
       <c r="J48" t="s" s="6">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K48" t="s" s="6">
         <v>24</v>
@@ -3039,29 +2955,29 @@
         <v>10</v>
       </c>
       <c r="M48" t="n" s="7">
-        <v>42885.48330418982</v>
+        <v>42913.43219875</v>
       </c>
       <c r="N48"/>
       <c r="O48" t="s" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P48" t="s" s="6">
-        <v>26</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="6">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B49" t="s" s="6">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C49" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="s" s="6">
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="F49" t="s" s="6">
         <v>20</v>
@@ -3071,10 +2987,10 @@
       </c>
       <c r="H49"/>
       <c r="I49" t="s" s="6">
-        <v>50</v>
+        <v>197</v>
       </c>
       <c r="J49" t="s" s="6">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="K49" t="s" s="6">
         <v>24</v>
@@ -3083,7 +2999,7 @@
         <v>10</v>
       </c>
       <c r="M49" t="n" s="7">
-        <v>42887.53432255787</v>
+        <v>42914.538412002315</v>
       </c>
       <c r="N49"/>
       <c r="O49" t="s" s="6">
@@ -3095,17 +3011,17 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="6">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B50" t="s" s="6">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s" s="6">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F50" t="s" s="6">
         <v>20</v>
@@ -3115,10 +3031,10 @@
       </c>
       <c r="H50"/>
       <c r="I50" t="s" s="6">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="J50" t="s" s="6">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="K50" t="s" s="6">
         <v>24</v>
@@ -3127,7 +3043,7 @@
         <v>10</v>
       </c>
       <c r="M50" t="n" s="7">
-        <v>42893.74893450231</v>
+        <v>42921.431484155095</v>
       </c>
       <c r="N50"/>
       <c r="O50" t="s" s="6">
@@ -3139,17 +3055,17 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="6">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B51" t="s" s="6">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="s" s="6">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="F51" t="s" s="6">
         <v>20</v>
@@ -3159,7 +3075,7 @@
       </c>
       <c r="H51"/>
       <c r="I51" t="s" s="6">
-        <v>69</v>
+        <v>204</v>
       </c>
       <c r="J51" t="s" s="6">
         <v>70</v>
@@ -3171,11 +3087,11 @@
         <v>10</v>
       </c>
       <c r="M51" t="n" s="7">
-        <v>42894.3833237037</v>
+        <v>42922.70177399305</v>
       </c>
       <c r="N51"/>
       <c r="O51" t="s" s="6">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="P51" t="s" s="6">
         <v>26</v>
@@ -3183,10 +3099,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="6">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s" s="6">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>18</v>
@@ -3203,10 +3119,10 @@
       </c>
       <c r="H52"/>
       <c r="I52" t="s" s="6">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="J52" t="s" s="6">
-        <v>46</v>
+        <v>208</v>
       </c>
       <c r="K52" t="s" s="6">
         <v>24</v>
@@ -3215,7 +3131,7 @@
         <v>10</v>
       </c>
       <c r="M52" t="n" s="7">
-        <v>42894.63695923611</v>
+        <v>42927.53268582176</v>
       </c>
       <c r="N52"/>
       <c r="O52" t="s" s="6">
@@ -3227,17 +3143,17 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="6">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s" s="6">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D53"/>
       <c r="E53" t="s" s="6">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F53" t="s" s="6">
         <v>20</v>
@@ -3247,10 +3163,10 @@
       </c>
       <c r="H53"/>
       <c r="I53" t="s" s="6">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="J53" t="s" s="6">
-        <v>31</v>
+        <v>201</v>
       </c>
       <c r="K53" t="s" s="6">
         <v>24</v>
@@ -3259,7 +3175,7 @@
         <v>10</v>
       </c>
       <c r="M53" t="n" s="7">
-        <v>42901.412132060184</v>
+        <v>42927.66715631945</v>
       </c>
       <c r="N53"/>
       <c r="O53" t="s" s="6">
@@ -3271,17 +3187,17 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="6">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s" s="6">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D54"/>
       <c r="E54" t="s" s="6">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="F54" t="s" s="6">
         <v>20</v>
@@ -3291,7 +3207,7 @@
       </c>
       <c r="H54"/>
       <c r="I54" t="s" s="6">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J54" t="s" s="6">
         <v>70</v>
@@ -3303,7 +3219,7 @@
         <v>10</v>
       </c>
       <c r="M54" t="n" s="7">
-        <v>42902.572656655095</v>
+        <v>42928.654776469906</v>
       </c>
       <c r="N54"/>
       <c r="O54" t="s" s="6">
@@ -3315,17 +3231,17 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="6">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s" s="6">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D55"/>
       <c r="E55" t="s" s="6">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F55" t="s" s="6">
         <v>20</v>
@@ -3335,10 +3251,10 @@
       </c>
       <c r="H55"/>
       <c r="I55" t="s" s="6">
-        <v>210</v>
+        <v>121</v>
       </c>
       <c r="J55" t="s" s="6">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="K55" t="s" s="6">
         <v>24</v>
@@ -3347,7 +3263,7 @@
         <v>10</v>
       </c>
       <c r="M55" t="n" s="7">
-        <v>42907.33971252315</v>
+        <v>42934.604348726854</v>
       </c>
       <c r="N55"/>
       <c r="O55" t="s" s="6">
@@ -3359,28 +3275,30 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="6">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="B56" t="s" s="6">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="C56" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D56"/>
       <c r="E56" t="s" s="6">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F56" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G56" t="s" s="6">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H56"/>
-      <c r="I56"/>
+      <c r="I56" t="s" s="6">
+        <v>207</v>
+      </c>
       <c r="J56" t="s" s="6">
-        <v>75</v>
+        <v>208</v>
       </c>
       <c r="K56" t="s" s="6">
         <v>24</v>
@@ -3389,29 +3307,29 @@
         <v>10</v>
       </c>
       <c r="M56" t="n" s="7">
-        <v>42913.43219875</v>
+        <v>42937.36092556713</v>
       </c>
       <c r="N56"/>
       <c r="O56" t="s" s="6">
         <v>25</v>
       </c>
       <c r="P56" t="s" s="6">
-        <v>214</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B57" t="s" s="6">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C57" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D57"/>
       <c r="E57" t="s" s="6">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="F57" t="s" s="6">
         <v>20</v>
@@ -3421,10 +3339,10 @@
       </c>
       <c r="H57"/>
       <c r="I57" t="s" s="6">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J57" t="s" s="6">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="K57" t="s" s="6">
         <v>24</v>
@@ -3433,7 +3351,7 @@
         <v>10</v>
       </c>
       <c r="M57" t="n" s="7">
-        <v>42914.538412002315</v>
+        <v>42940.655258287035</v>
       </c>
       <c r="N57"/>
       <c r="O57" t="s" s="6">
@@ -3445,17 +3363,17 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="6">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B58" t="s" s="6">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C58" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D58"/>
       <c r="E58" t="s" s="6">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F58" t="s" s="6">
         <v>20</v>
@@ -3465,10 +3383,10 @@
       </c>
       <c r="H58"/>
       <c r="I58" t="s" s="6">
-        <v>50</v>
+        <v>204</v>
       </c>
       <c r="J58" t="s" s="6">
-        <v>222</v>
+        <v>70</v>
       </c>
       <c r="K58" t="s" s="6">
         <v>24</v>
@@ -3477,7 +3395,7 @@
         <v>10</v>
       </c>
       <c r="M58" t="n" s="7">
-        <v>42921.431484155095</v>
+        <v>42941.4359131713</v>
       </c>
       <c r="N58"/>
       <c r="O58" t="s" s="6">
@@ -3489,17 +3407,17 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="6">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B59" t="s" s="6">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C59" t="s" s="6">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D59"/>
       <c r="E59" t="s" s="6">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="F59" t="s" s="6">
         <v>20</v>
@@ -3509,10 +3427,10 @@
       </c>
       <c r="H59"/>
       <c r="I59" t="s" s="6">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="J59" t="s" s="6">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="K59" t="s" s="6">
         <v>24</v>
@@ -3521,11 +3439,11 @@
         <v>10</v>
       </c>
       <c r="M59" t="n" s="7">
-        <v>42922.70177399305</v>
+        <v>42940.7480615625</v>
       </c>
       <c r="N59"/>
       <c r="O59" t="s" s="6">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="P59" t="s" s="6">
         <v>26</v>
@@ -3533,17 +3451,17 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="6">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B60" t="s" s="6">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C60" t="s" s="6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D60"/>
       <c r="E60" t="s" s="6">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="F60" t="s" s="6">
         <v>20</v>
@@ -3553,10 +3471,10 @@
       </c>
       <c r="H60"/>
       <c r="I60" t="s" s="6">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="J60" t="s" s="6">
-        <v>228</v>
+        <v>85</v>
       </c>
       <c r="K60" t="s" s="6">
         <v>24</v>
@@ -3565,11 +3483,11 @@
         <v>10</v>
       </c>
       <c r="M60" t="n" s="7">
-        <v>42927.53268582176</v>
+        <v>42941.46744346065</v>
       </c>
       <c r="N60"/>
       <c r="O60" t="s" s="6">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P60" t="s" s="6">
         <v>26</v>
@@ -3577,17 +3495,17 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="6">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B61" t="s" s="6">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C61" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D61"/>
       <c r="E61" t="s" s="6">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="F61" t="s" s="6">
         <v>20</v>
@@ -3597,10 +3515,10 @@
       </c>
       <c r="H61"/>
       <c r="I61" t="s" s="6">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="J61" t="s" s="6">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="K61" t="s" s="6">
         <v>24</v>
@@ -3609,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="M61" t="n" s="7">
-        <v>42927.66715631945</v>
+        <v>42942.628795069446</v>
       </c>
       <c r="N61"/>
       <c r="O61" t="s" s="6">
@@ -3621,30 +3539,28 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="6">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B62" t="s" s="6">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C62" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D62"/>
       <c r="E62" t="s" s="6">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F62" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G62" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H62"/>
-      <c r="I62" t="s" s="6">
-        <v>69</v>
-      </c>
+      <c r="I62"/>
       <c r="J62" t="s" s="6">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="K62" t="s" s="6">
         <v>24</v>
@@ -3653,7 +3569,7 @@
         <v>10</v>
       </c>
       <c r="M62" t="n" s="7">
-        <v>42928.654776469906</v>
+        <v>42942.61818179398</v>
       </c>
       <c r="N62"/>
       <c r="O62" t="s" s="6">
@@ -3665,17 +3581,17 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="6">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B63" t="s" s="6">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C63" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D63"/>
       <c r="E63" t="s" s="6">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F63" t="s" s="6">
         <v>20</v>
@@ -3685,10 +3601,10 @@
       </c>
       <c r="H63"/>
       <c r="I63" t="s" s="6">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="J63" t="s" s="6">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="K63" t="s" s="6">
         <v>24</v>
@@ -3697,7 +3613,7 @@
         <v>10</v>
       </c>
       <c r="M63" t="n" s="7">
-        <v>42930.60860648148</v>
+        <v>42943.78652796296</v>
       </c>
       <c r="N63"/>
       <c r="O63" t="s" s="6">
@@ -3709,30 +3625,28 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="6">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B64" t="s" s="6">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C64" t="s" s="6">
         <v>18</v>
       </c>
       <c r="D64"/>
       <c r="E64" t="s" s="6">
-        <v>241</v>
+        <v>126</v>
       </c>
       <c r="F64" t="s" s="6">
         <v>20</v>
       </c>
       <c r="G64" t="s" s="6">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H64"/>
-      <c r="I64" t="s" s="6">
-        <v>130</v>
-      </c>
+      <c r="I64"/>
       <c r="J64" t="s" s="6">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="K64" t="s" s="6">
         <v>24</v>
@@ -3741,7 +3655,7 @@
         <v>10</v>
       </c>
       <c r="M64" t="n" s="7">
-        <v>42934.604348726854</v>
+        <v>42944.452200405096</v>
       </c>
       <c r="N64"/>
       <c r="O64" t="s" s="6">
@@ -3751,484 +3665,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="s" s="6">
-        <v>242</v>
-      </c>
-      <c r="B65" t="s" s="6">
-        <v>243</v>
-      </c>
-      <c r="C65" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D65"/>
-      <c r="E65" t="s" s="6">
-        <v>244</v>
-      </c>
-      <c r="F65" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G65" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H65"/>
-      <c r="I65" t="s" s="6">
-        <v>227</v>
-      </c>
-      <c r="J65" t="s" s="6">
-        <v>228</v>
-      </c>
-      <c r="K65" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L65" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M65" t="n" s="7">
-        <v>42937.36092556713</v>
-      </c>
-      <c r="N65"/>
-      <c r="O65" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P65" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="6">
-        <v>245</v>
-      </c>
-      <c r="B66" t="s" s="6">
-        <v>246</v>
-      </c>
-      <c r="C66" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D66"/>
-      <c r="E66" t="s" s="6">
-        <v>247</v>
-      </c>
-      <c r="F66" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G66" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H66"/>
-      <c r="I66" t="s" s="6">
-        <v>248</v>
-      </c>
-      <c r="J66" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="K66" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L66" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M66" t="n" s="7">
-        <v>42940.655258287035</v>
-      </c>
-      <c r="N66"/>
-      <c r="O66" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P66" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="6">
-        <v>249</v>
-      </c>
-      <c r="B67" t="s" s="6">
-        <v>250</v>
-      </c>
-      <c r="C67" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D67"/>
-      <c r="E67" t="s" s="6">
-        <v>138</v>
-      </c>
-      <c r="F67" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G67" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H67"/>
-      <c r="I67" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="J67" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="K67" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L67" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M67" t="n" s="7">
-        <v>42940.7480615625</v>
-      </c>
-      <c r="N67"/>
-      <c r="O67" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="P67" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="6">
-        <v>251</v>
-      </c>
-      <c r="B68" t="s" s="6">
-        <v>252</v>
-      </c>
-      <c r="C68" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="D68"/>
-      <c r="E68" t="s" s="6">
-        <v>221</v>
-      </c>
-      <c r="F68" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G68" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H68"/>
-      <c r="I68" t="s" s="6">
-        <v>253</v>
-      </c>
-      <c r="J68" t="s" s="6">
-        <v>93</v>
-      </c>
-      <c r="K68" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L68" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M68" t="n" s="7">
-        <v>42941.46744346065</v>
-      </c>
-      <c r="N68"/>
-      <c r="O68" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="P68" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="6">
-        <v>254</v>
-      </c>
-      <c r="B69" t="s" s="6">
-        <v>255</v>
-      </c>
-      <c r="C69" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D69"/>
-      <c r="E69" t="s" s="6">
-        <v>221</v>
-      </c>
-      <c r="F69" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G69" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H69"/>
-      <c r="I69" t="s" s="6">
-        <v>227</v>
-      </c>
-      <c r="J69" t="s" s="6">
-        <v>228</v>
-      </c>
-      <c r="K69" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L69" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M69" t="n" s="7">
-        <v>42942.628795069446</v>
-      </c>
-      <c r="N69"/>
-      <c r="O69" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P69" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="6">
-        <v>256</v>
-      </c>
-      <c r="B70" t="s" s="6">
-        <v>257</v>
-      </c>
-      <c r="C70" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D70"/>
-      <c r="E70" t="s" s="6">
-        <v>258</v>
-      </c>
-      <c r="F70" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G70" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H70"/>
-      <c r="I70" t="s" s="6">
-        <v>89</v>
-      </c>
-      <c r="J70" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="K70" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L70" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M70" t="n" s="7">
-        <v>42942.52407478009</v>
-      </c>
-      <c r="N70"/>
-      <c r="O70" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P70" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="6">
-        <v>259</v>
-      </c>
-      <c r="B71" t="s" s="6">
-        <v>260</v>
-      </c>
-      <c r="C71" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D71"/>
-      <c r="E71" t="s" s="6">
-        <v>261</v>
-      </c>
-      <c r="F71" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G71" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="H71"/>
-      <c r="I71"/>
-      <c r="J71" t="s" s="6">
-        <v>46</v>
-      </c>
-      <c r="K71" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L71" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M71" t="n" s="7">
-        <v>42942.61818179398</v>
-      </c>
-      <c r="N71"/>
-      <c r="O71" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P71" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="6">
-        <v>262</v>
-      </c>
-      <c r="B72" t="s" s="6">
-        <v>263</v>
-      </c>
-      <c r="C72" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D72"/>
-      <c r="E72" t="s" s="6">
-        <v>142</v>
-      </c>
-      <c r="F72" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G72" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H72"/>
-      <c r="I72"/>
-      <c r="J72" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="K72" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L72" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M72" t="n" s="7">
-        <v>42943.44300207176</v>
-      </c>
-      <c r="N72"/>
-      <c r="O72" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P72" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="6">
-        <v>264</v>
-      </c>
-      <c r="B73" t="s" s="6">
-        <v>265</v>
-      </c>
-      <c r="C73" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D73"/>
-      <c r="E73" t="s" s="6">
-        <v>266</v>
-      </c>
-      <c r="F73" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G73" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="H73"/>
-      <c r="I73"/>
-      <c r="J73" t="s" s="6">
-        <v>70</v>
-      </c>
-      <c r="K73" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L73" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M73" t="n" s="7">
-        <v>42943.45755769676</v>
-      </c>
-      <c r="N73"/>
-      <c r="O73" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P73" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="6">
-        <v>267</v>
-      </c>
-      <c r="B74" t="s" s="6">
-        <v>268</v>
-      </c>
-      <c r="C74" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D74"/>
-      <c r="E74" t="s" s="6">
-        <v>137</v>
-      </c>
-      <c r="F74" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G74" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="H74"/>
-      <c r="I74"/>
-      <c r="J74" t="s" s="6">
-        <v>228</v>
-      </c>
-      <c r="K74" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L74" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M74" t="n" s="7">
-        <v>42943.71504658565</v>
-      </c>
-      <c r="N74"/>
-      <c r="O74" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P74" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="6">
-        <v>269</v>
-      </c>
-      <c r="B75" t="s" s="6">
-        <v>270</v>
-      </c>
-      <c r="C75" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D75"/>
-      <c r="E75" t="s" s="6">
-        <v>271</v>
-      </c>
-      <c r="F75" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="G75" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H75"/>
-      <c r="I75" t="s" s="6">
-        <v>218</v>
-      </c>
-      <c r="J75" t="s" s="6">
-        <v>238</v>
-      </c>
-      <c r="K75" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="L75" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="M75" t="n" s="7">
-        <v>42943.78652796296</v>
-      </c>
-      <c r="N75"/>
-      <c r="O75" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="P75" t="s" s="6">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P75"/>
+  <autoFilter ref="A1:P64"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>